<commit_message>
- Modified strings and start message; - Fixed bug when getting userId in /insert command.
</commit_message>
<xml_diff>
--- a/empty_sheet.xlsx
+++ b/empty_sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GENNAIO" sheetId="1" state="visible" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>MESE</t>
   </si>
@@ -35,13 +35,7 @@
     <t>LAVORATORE</t>
   </si>
   <si>
-    <t xml:space="preserve">Marcello Nobili</t>
-  </si>
-  <si>
     <t>RESPONSABILE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alexander Karelin</t>
   </si>
   <si>
     <t>GIORNO</t>
@@ -80,12 +74,6 @@
     <t>Sab</t>
   </si>
   <si>
-    <t>6,5</t>
-  </si>
-  <si>
-    <t>1,5</t>
-  </si>
-  <si>
     <t xml:space="preserve">TOTALE ORE</t>
   </si>
   <si>
@@ -101,13 +89,7 @@
     <t>MARZO</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>APRILE</t>
-  </si>
-  <si>
-    <t>1,75</t>
   </si>
   <si>
     <t>MAGGIO</t>
@@ -1241,9 +1223,7 @@
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="C4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="3"/>
@@ -1253,11 +1233,9 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3"/>
@@ -1266,19 +1244,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="D8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -1290,7 +1268,7 @@
     </row>
     <row r="10">
       <c r="A10" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
@@ -1301,59 +1279,51 @@
     </row>
     <row r="11">
       <c r="A11" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="19">
         <v>2</v>
       </c>
       <c r="C11" s="20"/>
-      <c r="D11" s="20">
-        <v>8</v>
-      </c>
+      <c r="D11" s="20"/>
       <c r="E11" s="21"/>
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="22">
         <v>3</v>
       </c>
       <c r="C12" s="23"/>
-      <c r="D12" s="23">
-        <v>8</v>
-      </c>
+      <c r="D12" s="23"/>
       <c r="E12" s="21"/>
     </row>
     <row r="13">
       <c r="A13" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="19">
         <v>4</v>
       </c>
       <c r="C13" s="20"/>
-      <c r="D13" s="20">
-        <v>8</v>
-      </c>
+      <c r="D13" s="20"/>
       <c r="E13" s="21"/>
     </row>
     <row r="14">
       <c r="A14" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="19">
         <v>5</v>
       </c>
       <c r="C14" s="24"/>
-      <c r="D14" s="24">
-        <v>8</v>
-      </c>
+      <c r="D14" s="24"/>
       <c r="E14" s="25"/>
     </row>
     <row r="15">
       <c r="A15" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="15">
         <v>6</v>
@@ -1364,7 +1334,7 @@
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="27">
         <v>7</v>
@@ -1375,7 +1345,7 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" s="27">
         <v>8</v>
@@ -1386,72 +1356,62 @@
     </row>
     <row r="18">
       <c r="A18" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="24">
         <v>9</v>
       </c>
-      <c r="C18" s="24">
-        <v>8</v>
-      </c>
+      <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19">
       <c r="A19" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" s="24">
         <v>10</v>
       </c>
-      <c r="C19" s="24">
-        <v>8</v>
-      </c>
+      <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20">
       <c r="A20" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" s="19">
         <v>11</v>
       </c>
-      <c r="C20" s="20">
-        <v>8</v>
-      </c>
+      <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
     </row>
     <row r="21">
       <c r="A21" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="19">
         <v>12</v>
       </c>
-      <c r="C21" s="20">
-        <v>8</v>
-      </c>
+      <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
     </row>
     <row r="22">
       <c r="A22" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="19">
         <v>13</v>
       </c>
-      <c r="C22" s="20">
-        <v>8</v>
-      </c>
+      <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
     </row>
     <row r="23">
       <c r="A23" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" s="27">
         <v>14</v>
@@ -1462,7 +1422,7 @@
     </row>
     <row r="24">
       <c r="A24" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B24" s="27">
         <v>15</v>
@@ -1473,74 +1433,62 @@
     </row>
     <row r="25">
       <c r="A25" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="24">
         <v>16</v>
       </c>
-      <c r="C25" s="24">
-        <v>8</v>
-      </c>
+      <c r="C25" s="24"/>
       <c r="D25" s="24"/>
       <c r="E25" s="29"/>
     </row>
     <row r="26">
       <c r="A26" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B26" s="24">
         <v>17</v>
       </c>
-      <c r="C26" s="24">
-        <v>8</v>
-      </c>
+      <c r="C26" s="24"/>
       <c r="D26" s="24"/>
       <c r="E26" s="29"/>
     </row>
     <row r="27">
       <c r="A27" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B27" s="19">
         <v>18</v>
       </c>
-      <c r="C27" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>19</v>
-      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="21"/>
     </row>
     <row r="28">
       <c r="A28" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B28" s="19">
         <v>19</v>
       </c>
-      <c r="C28" s="20">
-        <v>8</v>
-      </c>
+      <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
     </row>
     <row r="29">
       <c r="A29" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B29" s="19">
         <v>20</v>
       </c>
-      <c r="C29" s="20">
-        <v>8</v>
-      </c>
+      <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="21"/>
     </row>
     <row r="30">
       <c r="A30" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B30" s="27">
         <v>21</v>
@@ -1551,7 +1499,7 @@
     </row>
     <row r="31">
       <c r="A31" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B31" s="27">
         <v>22</v>
@@ -1562,72 +1510,62 @@
     </row>
     <row r="32">
       <c r="A32" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" s="24">
         <v>23</v>
       </c>
-      <c r="C32" s="24">
-        <v>8</v>
-      </c>
+      <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="29"/>
     </row>
     <row r="33">
       <c r="A33" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B33" s="24">
         <v>24</v>
       </c>
-      <c r="C33" s="24">
-        <v>8</v>
-      </c>
+      <c r="C33" s="24"/>
       <c r="D33" s="24"/>
       <c r="E33" s="29"/>
     </row>
     <row r="34">
       <c r="A34" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B34" s="19">
         <v>25</v>
       </c>
-      <c r="C34" s="20">
-        <v>8</v>
-      </c>
+      <c r="C34" s="20"/>
       <c r="D34" s="20"/>
       <c r="E34" s="21"/>
     </row>
     <row r="35">
       <c r="A35" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B35" s="19">
         <v>26</v>
       </c>
-      <c r="C35" s="20">
-        <v>8</v>
-      </c>
+      <c r="C35" s="20"/>
       <c r="D35" s="20"/>
       <c r="E35" s="21"/>
     </row>
     <row r="36">
       <c r="A36" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B36" s="19">
         <v>27</v>
       </c>
-      <c r="C36" s="20">
-        <v>8</v>
-      </c>
+      <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="21"/>
     </row>
     <row r="37">
       <c r="A37" s="30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" s="27">
         <v>28</v>
@@ -1638,7 +1576,7 @@
     </row>
     <row r="38">
       <c r="A38" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B38" s="27">
         <v>29</v>
@@ -1649,53 +1587,49 @@
     </row>
     <row r="39">
       <c r="A39" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B39" s="24">
         <v>30</v>
       </c>
-      <c r="C39" s="24">
-        <v>8</v>
-      </c>
+      <c r="C39" s="24"/>
       <c r="D39" s="24"/>
       <c r="E39" s="29"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40" s="32">
         <v>31</v>
       </c>
-      <c r="C40" s="32">
-        <v>8</v>
-      </c>
+      <c r="C40" s="32"/>
       <c r="D40" s="32"/>
       <c r="E40" s="33"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
-      <c r="C41" s="36" t="e">
+      <c r="C41" s="36">
         <f>C10+C11+C12+C13+C14+C15+C16+C17+C18+C19+C20+C21+C22+C23+C24+C25+C26+C27+C28+C29+C30+C31+C32+C33+C34+C35+C36+C37+C38+C39+C40</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
         <f>SUM(D10:D40)</f>
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -1889,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
@@ -1912,7 +1846,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1923,19 +1857,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -1947,7 +1881,7 @@
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="51">
         <v>1</v>
@@ -1958,7 +1892,7 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="45">
         <v>2</v>
@@ -1969,7 +1903,7 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="45">
         <v>3</v>
@@ -1980,7 +1914,7 @@
     </row>
     <row r="13">
       <c r="A13" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="45">
         <v>4</v>
@@ -1991,7 +1925,7 @@
     </row>
     <row r="14">
       <c r="A14" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="45">
         <v>5</v>
@@ -2002,7 +1936,7 @@
     </row>
     <row r="15">
       <c r="A15" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="45">
         <v>6</v>
@@ -2013,7 +1947,7 @@
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="51">
         <v>7</v>
@@ -2024,7 +1958,7 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" s="51">
         <v>8</v>
@@ -2035,7 +1969,7 @@
     </row>
     <row r="18">
       <c r="A18" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="45">
         <v>9</v>
@@ -2046,7 +1980,7 @@
     </row>
     <row r="19">
       <c r="A19" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" s="45">
         <v>10</v>
@@ -2057,7 +1991,7 @@
     </row>
     <row r="20">
       <c r="A20" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" s="45">
         <v>11</v>
@@ -2068,7 +2002,7 @@
     </row>
     <row r="21">
       <c r="A21" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="45">
         <v>12</v>
@@ -2079,7 +2013,7 @@
     </row>
     <row r="22">
       <c r="A22" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="45">
         <v>13</v>
@@ -2090,7 +2024,7 @@
     </row>
     <row r="23">
       <c r="A23" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" s="51">
         <v>14</v>
@@ -2101,7 +2035,7 @@
     </row>
     <row r="24">
       <c r="A24" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B24" s="51">
         <v>15</v>
@@ -2112,7 +2046,7 @@
     </row>
     <row r="25">
       <c r="A25" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="45">
         <v>16</v>
@@ -2123,7 +2057,7 @@
     </row>
     <row r="26">
       <c r="A26" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B26" s="45">
         <v>17</v>
@@ -2134,7 +2068,7 @@
     </row>
     <row r="27">
       <c r="A27" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B27" s="45">
         <v>18</v>
@@ -2145,7 +2079,7 @@
     </row>
     <row r="28">
       <c r="A28" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B28" s="45">
         <v>19</v>
@@ -2156,7 +2090,7 @@
     </row>
     <row r="29">
       <c r="A29" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B29" s="45">
         <v>20</v>
@@ -2167,7 +2101,7 @@
     </row>
     <row r="30">
       <c r="A30" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B30" s="51">
         <v>21</v>
@@ -2178,7 +2112,7 @@
     </row>
     <row r="31">
       <c r="A31" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B31" s="51">
         <v>22</v>
@@ -2189,7 +2123,7 @@
     </row>
     <row r="32">
       <c r="A32" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" s="45">
         <v>23</v>
@@ -2200,7 +2134,7 @@
     </row>
     <row r="33">
       <c r="A33" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B33" s="45">
         <v>24</v>
@@ -2211,7 +2145,7 @@
     </row>
     <row r="34">
       <c r="A34" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B34" s="45">
         <v>25</v>
@@ -2222,7 +2156,7 @@
     </row>
     <row r="35">
       <c r="A35" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B35" s="45">
         <v>26</v>
@@ -2233,7 +2167,7 @@
     </row>
     <row r="36">
       <c r="A36" s="60" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B36" s="45">
         <v>27</v>
@@ -2244,7 +2178,7 @@
     </row>
     <row r="37">
       <c r="A37" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" s="51">
         <v>28</v>
@@ -2255,7 +2189,7 @@
     </row>
     <row r="38">
       <c r="A38" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B38" s="51">
         <v>29</v>
@@ -2266,7 +2200,7 @@
     </row>
     <row r="39">
       <c r="A39" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B39" s="45">
         <v>30</v>
@@ -2277,7 +2211,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40" s="52">
         <v>31</v>
@@ -2288,7 +2222,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
@@ -2298,7 +2232,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -2308,7 +2242,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -2502,7 +2436,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -2525,7 +2459,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -2536,19 +2470,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -2560,7 +2494,7 @@
     </row>
     <row r="10">
       <c r="A10" s="56" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="56">
         <v>1</v>
@@ -2571,7 +2505,7 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="45">
         <v>2</v>
@@ -2582,7 +2516,7 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="45">
         <v>3</v>
@@ -2593,7 +2527,7 @@
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="51">
         <v>4</v>
@@ -2604,7 +2538,7 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="51">
         <v>5</v>
@@ -2615,7 +2549,7 @@
     </row>
     <row r="15">
       <c r="A15" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="45">
         <v>6</v>
@@ -2626,7 +2560,7 @@
     </row>
     <row r="16">
       <c r="A16" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="45">
         <v>7</v>
@@ -2637,7 +2571,7 @@
     </row>
     <row r="17">
       <c r="A17" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="45">
         <v>8</v>
@@ -2648,7 +2582,7 @@
     </row>
     <row r="18">
       <c r="A18" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="45">
         <v>9</v>
@@ -2659,7 +2593,7 @@
     </row>
     <row r="19">
       <c r="A19" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="45">
         <v>10</v>
@@ -2670,7 +2604,7 @@
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="51">
         <v>11</v>
@@ -2681,7 +2615,7 @@
     </row>
     <row r="21">
       <c r="A21" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21" s="51">
         <v>12</v>
@@ -2692,7 +2626,7 @@
     </row>
     <row r="22">
       <c r="A22" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="45">
         <v>13</v>
@@ -2703,7 +2637,7 @@
     </row>
     <row r="23">
       <c r="A23" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="45">
         <v>14</v>
@@ -2714,7 +2648,7 @@
     </row>
     <row r="24">
       <c r="A24" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24" s="45">
         <v>15</v>
@@ -2725,7 +2659,7 @@
     </row>
     <row r="25">
       <c r="A25" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="45">
         <v>16</v>
@@ -2736,7 +2670,7 @@
     </row>
     <row r="26">
       <c r="A26" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B26" s="45">
         <v>17</v>
@@ -2747,7 +2681,7 @@
     </row>
     <row r="27">
       <c r="A27" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B27" s="51">
         <v>18</v>
@@ -2758,7 +2692,7 @@
     </row>
     <row r="28">
       <c r="A28" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B28" s="51">
         <v>19</v>
@@ -2769,7 +2703,7 @@
     </row>
     <row r="29">
       <c r="A29" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="45">
         <v>20</v>
@@ -2780,7 +2714,7 @@
     </row>
     <row r="30">
       <c r="A30" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="45">
         <v>21</v>
@@ -2791,7 +2725,7 @@
     </row>
     <row r="31">
       <c r="A31" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B31" s="45">
         <v>22</v>
@@ -2802,7 +2736,7 @@
     </row>
     <row r="32">
       <c r="A32" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B32" s="45">
         <v>23</v>
@@ -2813,7 +2747,7 @@
     </row>
     <row r="33">
       <c r="A33" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B33" s="45">
         <v>24</v>
@@ -2824,7 +2758,7 @@
     </row>
     <row r="34">
       <c r="A34" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B34" s="51">
         <v>25</v>
@@ -2835,7 +2769,7 @@
     </row>
     <row r="35">
       <c r="A35" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B35" s="51">
         <v>26</v>
@@ -2846,7 +2780,7 @@
     </row>
     <row r="36">
       <c r="A36" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36" s="45">
         <v>27</v>
@@ -2857,7 +2791,7 @@
     </row>
     <row r="37">
       <c r="A37" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B37" s="45">
         <v>28</v>
@@ -2868,7 +2802,7 @@
     </row>
     <row r="38">
       <c r="A38" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B38" s="45">
         <v>29</v>
@@ -2879,7 +2813,7 @@
     </row>
     <row r="39">
       <c r="A39" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B39" s="45">
         <v>30</v>
@@ -2897,7 +2831,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
@@ -2907,7 +2841,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -2917,7 +2851,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -3111,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3134,7 +3068,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -3145,19 +3079,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -3169,7 +3103,7 @@
     </row>
     <row r="10">
       <c r="A10" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="45">
         <v>1</v>
@@ -3180,7 +3114,7 @@
     </row>
     <row r="11">
       <c r="A11" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="51">
         <v>2</v>
@@ -3191,7 +3125,7 @@
     </row>
     <row r="12">
       <c r="A12" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="51">
         <v>3</v>
@@ -3202,7 +3136,7 @@
     </row>
     <row r="13">
       <c r="A13" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="45">
         <v>4</v>
@@ -3213,7 +3147,7 @@
     </row>
     <row r="14">
       <c r="A14" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="45">
         <v>5</v>
@@ -3224,7 +3158,7 @@
     </row>
     <row r="15">
       <c r="A15" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="45">
         <v>6</v>
@@ -3235,7 +3169,7 @@
     </row>
     <row r="16">
       <c r="A16" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="45">
         <v>7</v>
@@ -3246,7 +3180,7 @@
     </row>
     <row r="17">
       <c r="A17" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="56">
         <v>8</v>
@@ -3257,7 +3191,7 @@
     </row>
     <row r="18">
       <c r="A18" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="51">
         <v>9</v>
@@ -3268,7 +3202,7 @@
     </row>
     <row r="19">
       <c r="A19" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" s="51">
         <v>10</v>
@@ -3279,7 +3213,7 @@
     </row>
     <row r="20">
       <c r="A20" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="45">
         <v>11</v>
@@ -3290,7 +3224,7 @@
     </row>
     <row r="21">
       <c r="A21" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="45">
         <v>12</v>
@@ -3301,7 +3235,7 @@
     </row>
     <row r="22">
       <c r="A22" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B22" s="45">
         <v>13</v>
@@ -3312,7 +3246,7 @@
     </row>
     <row r="23">
       <c r="A23" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B23" s="45">
         <v>14</v>
@@ -3323,7 +3257,7 @@
     </row>
     <row r="24">
       <c r="A24" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B24" s="45">
         <v>15</v>
@@ -3334,7 +3268,7 @@
     </row>
     <row r="25">
       <c r="A25" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B25" s="51">
         <v>16</v>
@@ -3345,7 +3279,7 @@
     </row>
     <row r="26">
       <c r="A26" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="51">
         <v>17</v>
@@ -3356,7 +3290,7 @@
     </row>
     <row r="27">
       <c r="A27" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="45">
         <v>18</v>
@@ -3367,7 +3301,7 @@
     </row>
     <row r="28">
       <c r="A28" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" s="45">
         <v>19</v>
@@ -3378,7 +3312,7 @@
     </row>
     <row r="29">
       <c r="A29" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B29" s="45">
         <v>20</v>
@@ -3389,7 +3323,7 @@
     </row>
     <row r="30">
       <c r="A30" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30" s="45">
         <v>21</v>
@@ -3400,7 +3334,7 @@
     </row>
     <row r="31">
       <c r="A31" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" s="45">
         <v>22</v>
@@ -3411,7 +3345,7 @@
     </row>
     <row r="32">
       <c r="A32" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B32" s="51">
         <v>23</v>
@@ -3422,7 +3356,7 @@
     </row>
     <row r="33">
       <c r="A33" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B33" s="51">
         <v>24</v>
@@ -3433,7 +3367,7 @@
     </row>
     <row r="34">
       <c r="A34" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34" s="56">
         <v>25</v>
@@ -3444,7 +3378,7 @@
     </row>
     <row r="35">
       <c r="A35" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B35" s="56">
         <v>26</v>
@@ -3455,7 +3389,7 @@
     </row>
     <row r="36">
       <c r="A36" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B36" s="45">
         <v>27</v>
@@ -3466,7 +3400,7 @@
     </row>
     <row r="37">
       <c r="A37" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B37" s="45">
         <v>28</v>
@@ -3477,7 +3411,7 @@
     </row>
     <row r="38">
       <c r="A38" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B38" s="45">
         <v>29</v>
@@ -3488,7 +3422,7 @@
     </row>
     <row r="39">
       <c r="A39" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B39" s="51">
         <v>30</v>
@@ -3499,7 +3433,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="61" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B40" s="62">
         <v>31</v>
@@ -3510,7 +3444,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
@@ -3520,7 +3454,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -3530,7 +3464,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -3724,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -3747,7 +3681,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="41"/>
     </row>
@@ -3758,19 +3692,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -3782,7 +3716,7 @@
     </row>
     <row r="10">
       <c r="A10" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="19">
         <v>1</v>
@@ -3793,7 +3727,7 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="19">
         <v>2</v>
@@ -3804,7 +3738,7 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="19">
         <v>3</v>
@@ -3815,7 +3749,7 @@
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="27">
         <v>4</v>
@@ -3826,7 +3760,7 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="27">
         <v>5</v>
@@ -3837,7 +3771,7 @@
     </row>
     <row r="15">
       <c r="A15" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="24">
         <v>6</v>
@@ -3848,7 +3782,7 @@
     </row>
     <row r="16">
       <c r="A16" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="19">
         <v>7</v>
@@ -3859,7 +3793,7 @@
     </row>
     <row r="17">
       <c r="A17" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="19">
         <v>8</v>
@@ -3870,7 +3804,7 @@
     </row>
     <row r="18">
       <c r="A18" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="19">
         <v>9</v>
@@ -3881,7 +3815,7 @@
     </row>
     <row r="19">
       <c r="A19" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="19">
         <v>10</v>
@@ -3892,7 +3826,7 @@
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="27">
         <v>11</v>
@@ -3903,7 +3837,7 @@
     </row>
     <row r="21">
       <c r="A21" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21" s="27">
         <v>12</v>
@@ -3914,7 +3848,7 @@
     </row>
     <row r="22">
       <c r="A22" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="24">
         <v>13</v>
@@ -3925,7 +3859,7 @@
     </row>
     <row r="23">
       <c r="A23" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="19">
         <v>14</v>
@@ -3936,7 +3870,7 @@
     </row>
     <row r="24">
       <c r="A24" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24" s="19">
         <v>15</v>
@@ -3947,7 +3881,7 @@
     </row>
     <row r="25">
       <c r="A25" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="19">
         <v>16</v>
@@ -3958,7 +3892,7 @@
     </row>
     <row r="26">
       <c r="A26" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B26" s="19">
         <v>17</v>
@@ -3969,7 +3903,7 @@
     </row>
     <row r="27">
       <c r="A27" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B27" s="27">
         <v>18</v>
@@ -3980,7 +3914,7 @@
     </row>
     <row r="28">
       <c r="A28" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B28" s="27">
         <v>19</v>
@@ -3991,7 +3925,7 @@
     </row>
     <row r="29">
       <c r="A29" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="24">
         <v>20</v>
@@ -4002,7 +3936,7 @@
     </row>
     <row r="30">
       <c r="A30" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="19">
         <v>21</v>
@@ -4013,7 +3947,7 @@
     </row>
     <row r="31">
       <c r="A31" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B31" s="19">
         <v>22</v>
@@ -4024,7 +3958,7 @@
     </row>
     <row r="32">
       <c r="A32" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B32" s="19">
         <v>23</v>
@@ -4035,7 +3969,7 @@
     </row>
     <row r="33">
       <c r="A33" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B33" s="19">
         <v>24</v>
@@ -4046,7 +3980,7 @@
     </row>
     <row r="34">
       <c r="A34" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B34" s="27">
         <v>25</v>
@@ -4057,7 +3991,7 @@
     </row>
     <row r="35">
       <c r="A35" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B35" s="27">
         <v>26</v>
@@ -4068,7 +4002,7 @@
     </row>
     <row r="36">
       <c r="A36" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36" s="24">
         <v>27</v>
@@ -4079,7 +4013,7 @@
     </row>
     <row r="37">
       <c r="A37" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B37" s="19">
         <v>28</v>
@@ -4111,7 +4045,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
@@ -4121,7 +4055,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -4131,7 +4065,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -4304,7 +4238,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -4325,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -4348,7 +4282,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -4359,19 +4293,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -4383,7 +4317,7 @@
     </row>
     <row r="10">
       <c r="A10" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="45">
         <v>1</v>
@@ -4394,7 +4328,7 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="45">
         <v>2</v>
@@ -4405,20 +4339,18 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="45">
         <v>3</v>
       </c>
-      <c r="C12" s="46" t="s">
-        <v>25</v>
-      </c>
+      <c r="C12" s="46"/>
       <c r="D12" s="46"/>
       <c r="E12" s="21"/>
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="51">
         <v>4</v>
@@ -4429,7 +4361,7 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="51">
         <v>5</v>
@@ -4440,7 +4372,7 @@
     </row>
     <row r="15">
       <c r="A15" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="45">
         <v>6</v>
@@ -4451,7 +4383,7 @@
     </row>
     <row r="16">
       <c r="A16" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="45">
         <v>7</v>
@@ -4462,7 +4394,7 @@
     </row>
     <row r="17">
       <c r="A17" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="45">
         <v>8</v>
@@ -4473,7 +4405,7 @@
     </row>
     <row r="18">
       <c r="A18" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="45">
         <v>9</v>
@@ -4484,7 +4416,7 @@
     </row>
     <row r="19">
       <c r="A19" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="45">
         <v>10</v>
@@ -4495,7 +4427,7 @@
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="51">
         <v>11</v>
@@ -4506,7 +4438,7 @@
     </row>
     <row r="21">
       <c r="A21" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21" s="51">
         <v>12</v>
@@ -4517,7 +4449,7 @@
     </row>
     <row r="22">
       <c r="A22" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="45">
         <v>13</v>
@@ -4528,7 +4460,7 @@
     </row>
     <row r="23">
       <c r="A23" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="45">
         <v>14</v>
@@ -4539,7 +4471,7 @@
     </row>
     <row r="24">
       <c r="A24" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24" s="45">
         <v>15</v>
@@ -4550,7 +4482,7 @@
     </row>
     <row r="25">
       <c r="A25" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="45">
         <v>16</v>
@@ -4561,7 +4493,7 @@
     </row>
     <row r="26">
       <c r="A26" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B26" s="45">
         <v>17</v>
@@ -4572,7 +4504,7 @@
     </row>
     <row r="27">
       <c r="A27" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B27" s="51">
         <v>18</v>
@@ -4583,7 +4515,7 @@
     </row>
     <row r="28">
       <c r="A28" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B28" s="51">
         <v>19</v>
@@ -4594,7 +4526,7 @@
     </row>
     <row r="29">
       <c r="A29" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="45">
         <v>20</v>
@@ -4605,7 +4537,7 @@
     </row>
     <row r="30">
       <c r="A30" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="45">
         <v>21</v>
@@ -4616,7 +4548,7 @@
     </row>
     <row r="31">
       <c r="A31" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B31" s="45">
         <v>22</v>
@@ -4627,7 +4559,7 @@
     </row>
     <row r="32">
       <c r="A32" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B32" s="45">
         <v>23</v>
@@ -4638,7 +4570,7 @@
     </row>
     <row r="33">
       <c r="A33" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B33" s="45">
         <v>24</v>
@@ -4649,7 +4581,7 @@
     </row>
     <row r="34">
       <c r="A34" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B34" s="51">
         <v>25</v>
@@ -4660,7 +4592,7 @@
     </row>
     <row r="35">
       <c r="A35" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B35" s="51">
         <v>26</v>
@@ -4671,7 +4603,7 @@
     </row>
     <row r="36">
       <c r="A36" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36" s="45">
         <v>27</v>
@@ -4682,7 +4614,7 @@
     </row>
     <row r="37">
       <c r="A37" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B37" s="45">
         <v>28</v>
@@ -4693,7 +4625,7 @@
     </row>
     <row r="38">
       <c r="A38" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B38" s="45">
         <v>29</v>
@@ -4704,7 +4636,7 @@
     </row>
     <row r="39">
       <c r="A39" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B39" s="45">
         <v>30</v>
@@ -4715,7 +4647,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="47" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B40" s="52">
         <v>31</v>
@@ -4726,17 +4658,17 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
         <f>C10+C11+C12+C13+C14+C15+C16+C17+C18+C19+C20+C21+C22+C23+C24+C25+C26+C27+C28+C29+C30+C31+C32+C33+C34+C35+C36+C37+C38+C39+C40</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -4746,7 +4678,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -4919,7 +4851,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -4940,7 +4872,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -4963,7 +4895,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -4974,19 +4906,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -4998,7 +4930,7 @@
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="51">
         <v>1</v>
@@ -5009,7 +4941,7 @@
     </row>
     <row r="11">
       <c r="A11" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="51">
         <v>2</v>
@@ -5020,20 +4952,18 @@
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="45">
         <v>3</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>27</v>
-      </c>
+      <c r="C12" s="24"/>
       <c r="D12" s="24"/>
       <c r="E12" s="29"/>
     </row>
     <row r="13">
       <c r="A13" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="45">
         <v>4</v>
@@ -5044,7 +4974,7 @@
     </row>
     <row r="14">
       <c r="A14" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="45">
         <v>5</v>
@@ -5055,7 +4985,7 @@
     </row>
     <row r="15">
       <c r="A15" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="45">
         <v>6</v>
@@ -5066,7 +4996,7 @@
     </row>
     <row r="16">
       <c r="A16" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="45">
         <v>7</v>
@@ -5077,7 +5007,7 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="51">
         <v>8</v>
@@ -5088,7 +5018,7 @@
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="15">
         <v>9</v>
@@ -5099,7 +5029,7 @@
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19" s="15">
         <v>10</v>
@@ -5110,7 +5040,7 @@
     </row>
     <row r="20">
       <c r="A20" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" s="45">
         <v>11</v>
@@ -5121,7 +5051,7 @@
     </row>
     <row r="21">
       <c r="A21" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" s="45">
         <v>12</v>
@@ -5132,7 +5062,7 @@
     </row>
     <row r="22">
       <c r="A22" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22" s="45">
         <v>13</v>
@@ -5143,7 +5073,7 @@
     </row>
     <row r="23">
       <c r="A23" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B23" s="45">
         <v>14</v>
@@ -5154,7 +5084,7 @@
     </row>
     <row r="24">
       <c r="A24" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B24" s="51">
         <v>15</v>
@@ -5165,7 +5095,7 @@
     </row>
     <row r="25">
       <c r="A25" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25" s="51">
         <v>16</v>
@@ -5176,7 +5106,7 @@
     </row>
     <row r="26">
       <c r="A26" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26" s="19">
         <v>17</v>
@@ -5187,7 +5117,7 @@
     </row>
     <row r="27">
       <c r="A27" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B27" s="19">
         <v>18</v>
@@ -5198,7 +5128,7 @@
     </row>
     <row r="28">
       <c r="A28" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B28" s="45">
         <v>19</v>
@@ -5209,7 +5139,7 @@
     </row>
     <row r="29">
       <c r="A29" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B29" s="45">
         <v>20</v>
@@ -5220,7 +5150,7 @@
     </row>
     <row r="30">
       <c r="A30" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B30" s="45">
         <v>21</v>
@@ -5231,7 +5161,7 @@
     </row>
     <row r="31">
       <c r="A31" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B31" s="51">
         <v>22</v>
@@ -5242,7 +5172,7 @@
     </row>
     <row r="32">
       <c r="A32" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B32" s="51">
         <v>23</v>
@@ -5253,7 +5183,7 @@
     </row>
     <row r="33">
       <c r="A33" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33" s="45">
         <v>24</v>
@@ -5264,7 +5194,7 @@
     </row>
     <row r="34">
       <c r="A34" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B34" s="15">
         <v>25</v>
@@ -5275,7 +5205,7 @@
     </row>
     <row r="35">
       <c r="A35" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B35" s="45">
         <v>26</v>
@@ -5286,7 +5216,7 @@
     </row>
     <row r="36">
       <c r="A36" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B36" s="45">
         <v>27</v>
@@ -5297,7 +5227,7 @@
     </row>
     <row r="37">
       <c r="A37" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B37" s="45">
         <v>28</v>
@@ -5308,7 +5238,7 @@
     </row>
     <row r="38">
       <c r="A38" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B38" s="51">
         <v>29</v>
@@ -5319,7 +5249,7 @@
     </row>
     <row r="39">
       <c r="A39" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B39" s="51">
         <v>30</v>
@@ -5337,17 +5267,17 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
-      <c r="C41" s="36" t="e">
+      <c r="C41" s="36">
         <f>C10+C11+C12+C13+C14+C15+C16+C17+C18+C19+C20+C21+C22+C23+C24+C25+C26+C27+C28+C29+C30+C31+C32+C33+C34+C35+C36+C37+C38+C39+C40</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -5357,7 +5287,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -5551,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -5574,7 +5504,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -5585,19 +5515,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -5609,7 +5539,7 @@
     </row>
     <row r="10">
       <c r="A10" s="55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="56">
         <v>1</v>
@@ -5620,7 +5550,7 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="45">
         <v>2</v>
@@ -5631,7 +5561,7 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="45">
         <v>3</v>
@@ -5642,7 +5572,7 @@
     </row>
     <row r="13">
       <c r="A13" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="45">
         <v>4</v>
@@ -5653,7 +5583,7 @@
     </row>
     <row r="14">
       <c r="A14" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="45">
         <v>5</v>
@@ -5664,7 +5594,7 @@
     </row>
     <row r="15">
       <c r="A15" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="51">
         <v>6</v>
@@ -5675,7 +5605,7 @@
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B16" s="51">
         <v>7</v>
@@ -5686,7 +5616,7 @@
     </row>
     <row r="17">
       <c r="A17" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17" s="45">
         <v>8</v>
@@ -5697,7 +5627,7 @@
     </row>
     <row r="18">
       <c r="A18" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18" s="45">
         <v>9</v>
@@ -5708,7 +5638,7 @@
     </row>
     <row r="19">
       <c r="A19" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B19" s="45">
         <v>10</v>
@@ -5719,7 +5649,7 @@
     </row>
     <row r="20">
       <c r="A20" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20" s="45">
         <v>11</v>
@@ -5730,7 +5660,7 @@
     </row>
     <row r="21">
       <c r="A21" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21" s="45">
         <v>12</v>
@@ -5741,7 +5671,7 @@
     </row>
     <row r="22">
       <c r="A22" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B22" s="51">
         <v>13</v>
@@ -5752,7 +5682,7 @@
     </row>
     <row r="23">
       <c r="A23" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23" s="51">
         <v>14</v>
@@ -5763,7 +5693,7 @@
     </row>
     <row r="24">
       <c r="A24" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" s="45">
         <v>15</v>
@@ -5774,7 +5704,7 @@
     </row>
     <row r="25">
       <c r="A25" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" s="45">
         <v>16</v>
@@ -5785,7 +5715,7 @@
     </row>
     <row r="26">
       <c r="A26" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B26" s="45">
         <v>17</v>
@@ -5796,7 +5726,7 @@
     </row>
     <row r="27">
       <c r="A27" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27" s="45">
         <v>18</v>
@@ -5807,7 +5737,7 @@
     </row>
     <row r="28">
       <c r="A28" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B28" s="45">
         <v>19</v>
@@ -5818,7 +5748,7 @@
     </row>
     <row r="29">
       <c r="A29" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B29" s="51">
         <v>20</v>
@@ -5829,7 +5759,7 @@
     </row>
     <row r="30">
       <c r="A30" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B30" s="51">
         <v>21</v>
@@ -5840,7 +5770,7 @@
     </row>
     <row r="31">
       <c r="A31" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" s="45">
         <v>22</v>
@@ -5851,7 +5781,7 @@
     </row>
     <row r="32">
       <c r="A32" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B32" s="45">
         <v>23</v>
@@ -5862,7 +5792,7 @@
     </row>
     <row r="33">
       <c r="A33" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B33" s="45">
         <v>24</v>
@@ -5873,7 +5803,7 @@
     </row>
     <row r="34">
       <c r="A34" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" s="45">
         <v>25</v>
@@ -5884,7 +5814,7 @@
     </row>
     <row r="35">
       <c r="A35" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="45">
         <v>26</v>
@@ -5895,7 +5825,7 @@
     </row>
     <row r="36">
       <c r="A36" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B36" s="51">
         <v>27</v>
@@ -5906,7 +5836,7 @@
     </row>
     <row r="37">
       <c r="A37" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B37" s="51">
         <v>28</v>
@@ -5917,7 +5847,7 @@
     </row>
     <row r="38">
       <c r="A38" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38" s="45">
         <v>29</v>
@@ -5928,7 +5858,7 @@
     </row>
     <row r="39">
       <c r="A39" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B39" s="45">
         <v>30</v>
@@ -5939,7 +5869,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="47" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B40" s="52">
         <v>31</v>
@@ -5950,7 +5880,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
@@ -5960,7 +5890,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -5970,7 +5900,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -6164,7 +6094,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -6187,7 +6117,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -6198,19 +6128,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -6222,7 +6152,7 @@
     </row>
     <row r="10">
       <c r="A10" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="45">
         <v>1</v>
@@ -6233,7 +6163,7 @@
     </row>
     <row r="11">
       <c r="A11" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="56">
         <v>2</v>
@@ -6244,7 +6174,7 @@
     </row>
     <row r="12">
       <c r="A12" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="51">
         <v>3</v>
@@ -6255,7 +6185,7 @@
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="51">
         <v>4</v>
@@ -6266,7 +6196,7 @@
     </row>
     <row r="14">
       <c r="A14" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="45">
         <v>5</v>
@@ -6277,7 +6207,7 @@
     </row>
     <row r="15">
       <c r="A15" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="45">
         <v>6</v>
@@ -6288,7 +6218,7 @@
     </row>
     <row r="16">
       <c r="A16" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="45">
         <v>7</v>
@@ -6299,7 +6229,7 @@
     </row>
     <row r="17">
       <c r="A17" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="45">
         <v>8</v>
@@ -6310,7 +6240,7 @@
     </row>
     <row r="18">
       <c r="A18" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="45">
         <v>9</v>
@@ -6321,7 +6251,7 @@
     </row>
     <row r="19">
       <c r="A19" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" s="51">
         <v>10</v>
@@ -6332,7 +6262,7 @@
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" s="51">
         <v>11</v>
@@ -6343,7 +6273,7 @@
     </row>
     <row r="21">
       <c r="A21" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" s="45">
         <v>12</v>
@@ -6354,7 +6284,7 @@
     </row>
     <row r="22">
       <c r="A22" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B22" s="45">
         <v>13</v>
@@ -6365,7 +6295,7 @@
     </row>
     <row r="23">
       <c r="A23" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23" s="45">
         <v>14</v>
@@ -6376,7 +6306,7 @@
     </row>
     <row r="24">
       <c r="A24" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B24" s="45">
         <v>15</v>
@@ -6387,7 +6317,7 @@
     </row>
     <row r="25">
       <c r="A25" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B25" s="45">
         <v>16</v>
@@ -6398,7 +6328,7 @@
     </row>
     <row r="26">
       <c r="A26" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B26" s="51">
         <v>17</v>
@@ -6409,7 +6339,7 @@
     </row>
     <row r="27">
       <c r="A27" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B27" s="51">
         <v>18</v>
@@ -6420,7 +6350,7 @@
     </row>
     <row r="28">
       <c r="A28" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="45">
         <v>19</v>
@@ -6431,7 +6361,7 @@
     </row>
     <row r="29">
       <c r="A29" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B29" s="45">
         <v>20</v>
@@ -6442,7 +6372,7 @@
     </row>
     <row r="30">
       <c r="A30" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B30" s="45">
         <v>21</v>
@@ -6453,7 +6383,7 @@
     </row>
     <row r="31">
       <c r="A31" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B31" s="45">
         <v>22</v>
@@ -6464,7 +6394,7 @@
     </row>
     <row r="32">
       <c r="A32" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B32" s="45">
         <v>23</v>
@@ -6475,7 +6405,7 @@
     </row>
     <row r="33">
       <c r="A33" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B33" s="51">
         <v>24</v>
@@ -6486,7 +6416,7 @@
     </row>
     <row r="34">
       <c r="A34" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B34" s="51">
         <v>25</v>
@@ -6497,7 +6427,7 @@
     </row>
     <row r="35">
       <c r="A35" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B35" s="45">
         <v>26</v>
@@ -6508,7 +6438,7 @@
     </row>
     <row r="36">
       <c r="A36" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B36" s="45">
         <v>27</v>
@@ -6519,7 +6449,7 @@
     </row>
     <row r="37">
       <c r="A37" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B37" s="45">
         <v>28</v>
@@ -6530,7 +6460,7 @@
     </row>
     <row r="38">
       <c r="A38" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B38" s="45">
         <v>29</v>
@@ -6541,7 +6471,7 @@
     </row>
     <row r="39">
       <c r="A39" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B39" s="45">
         <v>30</v>
@@ -6559,7 +6489,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
@@ -6569,7 +6499,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -6579,7 +6509,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -6773,7 +6703,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
@@ -6796,7 +6726,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="41"/>
     </row>
@@ -6807,19 +6737,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -6831,7 +6761,7 @@
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="51">
         <v>1</v>
@@ -6842,7 +6772,7 @@
     </row>
     <row r="11">
       <c r="A11" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="51">
         <v>2</v>
@@ -6853,7 +6783,7 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="45">
         <v>3</v>
@@ -6864,7 +6794,7 @@
     </row>
     <row r="13">
       <c r="A13" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="45">
         <v>4</v>
@@ -6875,7 +6805,7 @@
     </row>
     <row r="14">
       <c r="A14" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="45">
         <v>5</v>
@@ -6886,7 +6816,7 @@
     </row>
     <row r="15">
       <c r="A15" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="45">
         <v>6</v>
@@ -6897,7 +6827,7 @@
     </row>
     <row r="16">
       <c r="A16" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="45">
         <v>7</v>
@@ -6908,7 +6838,7 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="51">
         <v>8</v>
@@ -6919,7 +6849,7 @@
     </row>
     <row r="18">
       <c r="A18" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="51">
         <v>9</v>
@@ -6930,7 +6860,7 @@
     </row>
     <row r="19">
       <c r="A19" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19" s="45">
         <v>10</v>
@@ -6941,7 +6871,7 @@
     </row>
     <row r="20">
       <c r="A20" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" s="45">
         <v>11</v>
@@ -6952,7 +6882,7 @@
     </row>
     <row r="21">
       <c r="A21" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" s="45">
         <v>12</v>
@@ -6963,7 +6893,7 @@
     </row>
     <row r="22">
       <c r="A22" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22" s="45">
         <v>13</v>
@@ -6974,7 +6904,7 @@
     </row>
     <row r="23">
       <c r="A23" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B23" s="45">
         <v>14</v>
@@ -6985,7 +6915,7 @@
     </row>
     <row r="24">
       <c r="A24" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B24" s="51">
         <v>15</v>
@@ -6996,7 +6926,7 @@
     </row>
     <row r="25">
       <c r="A25" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25" s="51">
         <v>16</v>
@@ -7007,7 +6937,7 @@
     </row>
     <row r="26">
       <c r="A26" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26" s="45">
         <v>17</v>
@@ -7018,7 +6948,7 @@
     </row>
     <row r="27">
       <c r="A27" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B27" s="45">
         <v>18</v>
@@ -7029,7 +6959,7 @@
     </row>
     <row r="28">
       <c r="A28" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B28" s="45">
         <v>19</v>
@@ -7040,7 +6970,7 @@
     </row>
     <row r="29">
       <c r="A29" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B29" s="45">
         <v>20</v>
@@ -7051,7 +6981,7 @@
     </row>
     <row r="30">
       <c r="A30" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B30" s="45">
         <v>21</v>
@@ -7062,7 +6992,7 @@
     </row>
     <row r="31">
       <c r="A31" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B31" s="51">
         <v>22</v>
@@ -7073,7 +7003,7 @@
     </row>
     <row r="32">
       <c r="A32" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B32" s="51">
         <v>23</v>
@@ -7084,7 +7014,7 @@
     </row>
     <row r="33">
       <c r="A33" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33" s="45">
         <v>24</v>
@@ -7095,7 +7025,7 @@
     </row>
     <row r="34">
       <c r="A34" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B34" s="45">
         <v>25</v>
@@ -7106,7 +7036,7 @@
     </row>
     <row r="35">
       <c r="A35" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B35" s="45">
         <v>26</v>
@@ -7117,7 +7047,7 @@
     </row>
     <row r="36">
       <c r="A36" s="58" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B36" s="45">
         <v>27</v>
@@ -7128,7 +7058,7 @@
     </row>
     <row r="37">
       <c r="A37" s="58" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B37" s="45">
         <v>28</v>
@@ -7139,7 +7069,7 @@
     </row>
     <row r="38">
       <c r="A38" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B38" s="51">
         <v>29</v>
@@ -7150,7 +7080,7 @@
     </row>
     <row r="39">
       <c r="A39" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B39" s="51">
         <v>30</v>
@@ -7161,7 +7091,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B40" s="52">
         <v>31</v>
@@ -7172,7 +7102,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
@@ -7182,7 +7112,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -7192,7 +7122,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -7386,7 +7316,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -7409,7 +7339,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -7420,19 +7350,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -7444,7 +7374,7 @@
     </row>
     <row r="10">
       <c r="A10" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="45">
         <v>1</v>
@@ -7455,7 +7385,7 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="45">
         <v>2</v>
@@ -7466,7 +7396,7 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="45">
         <v>3</v>
@@ -7477,7 +7407,7 @@
     </row>
     <row r="13">
       <c r="A13" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="45">
         <v>4</v>
@@ -7488,7 +7418,7 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="51">
         <v>5</v>
@@ -7499,7 +7429,7 @@
     </row>
     <row r="15">
       <c r="A15" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" s="51">
         <v>6</v>
@@ -7510,7 +7440,7 @@
     </row>
     <row r="16">
       <c r="A16" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="45">
         <v>7</v>
@@ -7521,7 +7451,7 @@
     </row>
     <row r="17">
       <c r="A17" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" s="45">
         <v>8</v>
@@ -7532,7 +7462,7 @@
     </row>
     <row r="18">
       <c r="A18" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="45">
         <v>9</v>
@@ -7543,7 +7473,7 @@
     </row>
     <row r="19">
       <c r="A19" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" s="45">
         <v>10</v>
@@ -7554,7 +7484,7 @@
     </row>
     <row r="20">
       <c r="A20" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" s="45">
         <v>11</v>
@@ -7565,7 +7495,7 @@
     </row>
     <row r="21">
       <c r="A21" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" s="51">
         <v>12</v>
@@ -7576,7 +7506,7 @@
     </row>
     <row r="22">
       <c r="A22" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22" s="51">
         <v>13</v>
@@ -7587,7 +7517,7 @@
     </row>
     <row r="23">
       <c r="A23" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23" s="45">
         <v>14</v>
@@ -7598,7 +7528,7 @@
     </row>
     <row r="24">
       <c r="A24" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24" s="56">
         <v>15</v>
@@ -7609,7 +7539,7 @@
     </row>
     <row r="25">
       <c r="A25" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B25" s="56">
         <v>16</v>
@@ -7620,7 +7550,7 @@
     </row>
     <row r="26">
       <c r="A26" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26" s="45">
         <v>17</v>
@@ -7631,7 +7561,7 @@
     </row>
     <row r="27">
       <c r="A27" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B27" s="45">
         <v>18</v>
@@ -7642,7 +7572,7 @@
     </row>
     <row r="28">
       <c r="A28" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B28" s="51">
         <v>19</v>
@@ -7653,7 +7583,7 @@
     </row>
     <row r="29">
       <c r="A29" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B29" s="51">
         <v>20</v>
@@ -7664,7 +7594,7 @@
     </row>
     <row r="30">
       <c r="A30" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" s="45">
         <v>21</v>
@@ -7675,7 +7605,7 @@
     </row>
     <row r="31">
       <c r="A31" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B31" s="45">
         <v>22</v>
@@ -7686,7 +7616,7 @@
     </row>
     <row r="32">
       <c r="A32" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" s="45">
         <v>23</v>
@@ -7697,7 +7627,7 @@
     </row>
     <row r="33">
       <c r="A33" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B33" s="45">
         <v>24</v>
@@ -7708,7 +7638,7 @@
     </row>
     <row r="34">
       <c r="A34" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B34" s="45">
         <v>25</v>
@@ -7719,7 +7649,7 @@
     </row>
     <row r="35">
       <c r="A35" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B35" s="51">
         <v>26</v>
@@ -7730,7 +7660,7 @@
     </row>
     <row r="36">
       <c r="A36" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B36" s="51">
         <v>27</v>
@@ -7741,7 +7671,7 @@
     </row>
     <row r="37">
       <c r="A37" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B37" s="45">
         <v>28</v>
@@ -7752,7 +7682,7 @@
     </row>
     <row r="38">
       <c r="A38" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B38" s="45">
         <v>29</v>
@@ -7763,7 +7693,7 @@
     </row>
     <row r="39">
       <c r="A39" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B39" s="45">
         <v>30</v>
@@ -7774,7 +7704,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="59" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B40" s="52">
         <v>31</v>
@@ -7785,7 +7715,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
@@ -7795,7 +7725,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -7805,7 +7735,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">
@@ -7999,7 +7929,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
@@ -8022,7 +7952,7 @@
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -8033,19 +7963,19 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -8057,7 +7987,7 @@
     </row>
     <row r="10">
       <c r="A10" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="45">
         <v>1</v>
@@ -8068,7 +7998,7 @@
     </row>
     <row r="11">
       <c r="A11" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="51">
         <v>2</v>
@@ -8079,7 +8009,7 @@
     </row>
     <row r="12">
       <c r="A12" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="51">
         <v>3</v>
@@ -8090,7 +8020,7 @@
     </row>
     <row r="13">
       <c r="A13" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="45">
         <v>4</v>
@@ -8101,7 +8031,7 @@
     </row>
     <row r="14">
       <c r="A14" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="45">
         <v>5</v>
@@ -8112,7 +8042,7 @@
     </row>
     <row r="15">
       <c r="A15" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="45">
         <v>6</v>
@@ -8123,7 +8053,7 @@
     </row>
     <row r="16">
       <c r="A16" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="45">
         <v>7</v>
@@ -8134,7 +8064,7 @@
     </row>
     <row r="17">
       <c r="A17" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="45">
         <v>8</v>
@@ -8145,7 +8075,7 @@
     </row>
     <row r="18">
       <c r="A18" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="51">
         <v>9</v>
@@ -8156,7 +8086,7 @@
     </row>
     <row r="19">
       <c r="A19" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" s="51">
         <v>10</v>
@@ -8167,7 +8097,7 @@
     </row>
     <row r="20">
       <c r="A20" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="45">
         <v>11</v>
@@ -8178,7 +8108,7 @@
     </row>
     <row r="21">
       <c r="A21" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="45">
         <v>12</v>
@@ -8189,7 +8119,7 @@
     </row>
     <row r="22">
       <c r="A22" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B22" s="45">
         <v>13</v>
@@ -8200,7 +8130,7 @@
     </row>
     <row r="23">
       <c r="A23" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B23" s="45">
         <v>14</v>
@@ -8211,7 +8141,7 @@
     </row>
     <row r="24">
       <c r="A24" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B24" s="45">
         <v>15</v>
@@ -8222,7 +8152,7 @@
     </row>
     <row r="25">
       <c r="A25" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B25" s="51">
         <v>16</v>
@@ -8233,7 +8163,7 @@
     </row>
     <row r="26">
       <c r="A26" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="51">
         <v>17</v>
@@ -8244,7 +8174,7 @@
     </row>
     <row r="27">
       <c r="A27" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="45">
         <v>18</v>
@@ -8255,7 +8185,7 @@
     </row>
     <row r="28">
       <c r="A28" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" s="45">
         <v>19</v>
@@ -8266,7 +8196,7 @@
     </row>
     <row r="29">
       <c r="A29" s="44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B29" s="45">
         <v>20</v>
@@ -8277,7 +8207,7 @@
     </row>
     <row r="30">
       <c r="A30" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30" s="45">
         <v>21</v>
@@ -8288,7 +8218,7 @@
     </row>
     <row r="31">
       <c r="A31" s="44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" s="45">
         <v>22</v>
@@ -8299,7 +8229,7 @@
     </row>
     <row r="32">
       <c r="A32" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B32" s="51">
         <v>23</v>
@@ -8310,7 +8240,7 @@
     </row>
     <row r="33">
       <c r="A33" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B33" s="51">
         <v>24</v>
@@ -8321,7 +8251,7 @@
     </row>
     <row r="34">
       <c r="A34" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34" s="45">
         <v>25</v>
@@ -8332,7 +8262,7 @@
     </row>
     <row r="35">
       <c r="A35" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B35" s="45">
         <v>26</v>
@@ -8343,7 +8273,7 @@
     </row>
     <row r="36">
       <c r="A36" s="60" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B36" s="45">
         <v>27</v>
@@ -8354,7 +8284,7 @@
     </row>
     <row r="37">
       <c r="A37" s="60" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B37" s="45">
         <v>28</v>
@@ -8365,7 +8295,7 @@
     </row>
     <row r="38">
       <c r="A38" s="60" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B38" s="45">
         <v>29</v>
@@ -8376,7 +8306,7 @@
     </row>
     <row r="39">
       <c r="A39" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B39" s="51">
         <v>30</v>
@@ -8394,7 +8324,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B41" s="35"/>
       <c r="C41" s="36">
@@ -8404,7 +8334,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="39">
@@ -8414,7 +8344,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="39">

</xml_diff>